<commit_message>
Opportunities & Engagement - 1st Merge - 12 Mar 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTI0054719_VerificationOfNewFieldAssociatedOpportunityAvailabiltyAndFunctionalityOnCFOpportunityAndEngagementPage.xlsx
+++ b/TestData/LV_TMTI0054719_VerificationOfNewFieldAssociatedOpportunityAvailabiltyAndFunctionalityOnCFOpportunityAndEngagementPage.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4D8148-A907-4F5F-A19A-6205B91D1B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889E087C-AEED-40F8-B858-F9634BBC5CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D381DC3E-0C7A-48CF-8E3B-36CB765DCADA}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
-    <sheet name="AppName" sheetId="6" r:id="rId2"/>
-    <sheet name="ModuleName" sheetId="7" r:id="rId3"/>
-    <sheet name="Users" sheetId="2" r:id="rId4"/>
+    <sheet name="Users" sheetId="2" r:id="rId1"/>
+    <sheet name="AddOpportunity" sheetId="1" r:id="rId2"/>
+    <sheet name="AppName" sheetId="6" r:id="rId3"/>
+    <sheet name="ModuleName" sheetId="7" r:id="rId4"/>
     <sheet name="AddContact" sheetId="3" r:id="rId5"/>
     <sheet name="AssociatedOpp" sheetId="4" r:id="rId6"/>
     <sheet name="AssociatedEng" sheetId="5" r:id="rId7"/>
@@ -275,14 +275,14 @@
     <t>IndustryGroup/HLSector</t>
   </si>
   <si>
-    <t>CSDN-0000002536</t>
+    <t>BUS - Business Services</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,16 +298,211 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="62"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -315,9 +510,153 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="63"/>
+      </left>
+      <right style="double">
+        <color indexed="63"/>
+      </right>
+      <top style="double">
+        <color indexed="63"/>
+      </top>
+      <bottom style="double">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="44"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="52"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="49"/>
+      </top>
+      <bottom style="double">
+        <color indexed="49"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyFont="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyFont="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyFont="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyFont="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyFont="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -327,8 +666,50 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{70532A5E-ED7B-4B50-B732-AE68FFF61839}"/>
+    <cellStyle name="20% - Accent2 2" xfId="7" xr:uid="{2A44D02B-FED0-4045-8E4D-57B10437D4DC}"/>
+    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{46C7922A-55E3-4707-9F0D-47E7EB716B2D}"/>
+    <cellStyle name="20% - Accent4 2" xfId="4" xr:uid="{CC1C9AEA-E8C4-4F11-A910-C0D2765B73A4}"/>
+    <cellStyle name="20% - Accent5 2" xfId="5" xr:uid="{EA0FCE14-86F0-4AAC-A665-CCBEF4A77CE5}"/>
+    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{4E7FE761-97BB-40DB-9D85-516C09D32ED9}"/>
+    <cellStyle name="40% - Accent1 2" xfId="9" xr:uid="{975BCF06-2EBA-41BA-A79C-D6CF3AEDE862}"/>
+    <cellStyle name="40% - Accent2 2" xfId="7" xr:uid="{4B979877-2493-4804-927C-DB3B650091CA}"/>
+    <cellStyle name="40% - Accent3 2" xfId="8" xr:uid="{1D54709C-E269-4F1F-A8DF-E32A875C84F0}"/>
+    <cellStyle name="40% - Accent4 2" xfId="10" xr:uid="{C806437E-36E0-4767-9A8A-17989A761FAE}"/>
+    <cellStyle name="40% - Accent5 2" xfId="9" xr:uid="{B2F62248-4E13-4170-8CC1-2BDD0AA5F800}"/>
+    <cellStyle name="40% - Accent6 2" xfId="10" xr:uid="{99C9387F-CCB8-4263-9D1F-D33E35BD6DE5}"/>
+    <cellStyle name="60% - Accent1 2" xfId="11" xr:uid="{4855B05E-0695-4A8D-A936-95CDBB65EE29}"/>
+    <cellStyle name="60% - Accent2 2" xfId="12" xr:uid="{1BD04650-8BCF-48D7-A387-E154B0D0312D}"/>
+    <cellStyle name="60% - Accent3 2" xfId="13" xr:uid="{9A446298-4FA7-4414-ADC4-4E13640F4C77}"/>
+    <cellStyle name="60% - Accent4 2" xfId="14" xr:uid="{631E9A43-01A1-4F4D-9BC0-F0612781BB76}"/>
+    <cellStyle name="60% - Accent5 2" xfId="15" xr:uid="{6B7E3150-825C-4B81-90AF-1622FB2EE336}"/>
+    <cellStyle name="60% - Accent6 2" xfId="20" xr:uid="{B97C30B2-5BA8-4199-98BB-8F921E4BBCC6}"/>
+    <cellStyle name="Accent1 2" xfId="15" xr:uid="{139F6612-BDD4-437B-AC4A-15121D6084CA}"/>
+    <cellStyle name="Accent2 2" xfId="16" xr:uid="{4AA54995-FDCF-44BA-9833-67EC2FCF8478}"/>
+    <cellStyle name="Accent3 2" xfId="17" xr:uid="{47DFB160-ADB1-45C8-95AD-9458C3CA5894}"/>
+    <cellStyle name="Accent4 2" xfId="18" xr:uid="{6FE38665-220C-4770-AA6F-5776CFC5EA14}"/>
+    <cellStyle name="Accent5 2" xfId="19" xr:uid="{EC7D3441-C740-44C5-9173-0DFBA41A81E2}"/>
+    <cellStyle name="Accent6 2" xfId="20" xr:uid="{CFC3196C-BF3F-4F60-BE54-26F6586E6CAD}"/>
+    <cellStyle name="Bad 2" xfId="21" xr:uid="{595547C2-3AD8-4C61-8E94-C6E84A00225A}"/>
+    <cellStyle name="Calculation 2" xfId="22" xr:uid="{D012F96E-B051-49D7-97B7-035619B34E76}"/>
+    <cellStyle name="Check Cell 2" xfId="23" xr:uid="{D6EF1E26-E3FF-4E67-96F1-4F7CD75093BE}"/>
+    <cellStyle name="Explanatory Text 2" xfId="24" xr:uid="{1E72B956-568F-4C4E-A727-5022B04C494A}"/>
+    <cellStyle name="Good 2" xfId="25" xr:uid="{A4E65940-DB12-4044-BBE5-937370F50588}"/>
+    <cellStyle name="Heading 1 2" xfId="26" xr:uid="{12D0BCFA-32AB-49E8-86C0-F60087C26417}"/>
+    <cellStyle name="Heading 2 2" xfId="27" xr:uid="{563335C1-7A46-4549-A436-5B37293FB82D}"/>
+    <cellStyle name="Heading 3 2" xfId="28" xr:uid="{231820EB-570C-47BE-AF59-DAE85413D56C}"/>
+    <cellStyle name="Heading 4 2" xfId="29" xr:uid="{E31ABADC-E412-492B-83D1-B5E9D32C94D0}"/>
+    <cellStyle name="Input 2" xfId="30" xr:uid="{323DB55D-0DEE-4D4D-856F-F388DE2AAA20}"/>
+    <cellStyle name="Linked Cell 2" xfId="31" xr:uid="{C6EFD52E-F3FE-4743-94F5-3110873AA5BD}"/>
+    <cellStyle name="Neutral 2" xfId="32" xr:uid="{513F0FAB-2B43-4701-B495-8CCB93DE2866}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7C31C764-70E4-4DE7-A94A-406A1D7CD858}"/>
+    <cellStyle name="Note 2" xfId="33" xr:uid="{DB638097-0A1D-456B-867B-6648598D8289}"/>
+    <cellStyle name="Output 2" xfId="34" xr:uid="{92EB4E44-804D-4434-A696-ED6913ED7E41}"/>
+    <cellStyle name="Title 2" xfId="35" xr:uid="{AF000633-B37E-4F7F-8839-35999EB99CE0}"/>
+    <cellStyle name="Total 2" xfId="36" xr:uid="{D363E27D-2657-4401-B5F6-629E5784991E}"/>
+    <cellStyle name="Warning Text 2" xfId="37" xr:uid="{681E2417-CC62-48AC-9F03-C4A1BA375D9C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -639,200 +1020,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDA40C-CB43-498D-A2ED-A0851564593B}">
-  <dimension ref="A1:AD2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A3F6A9-43ED-49B3-9AC1-A223C8D04358}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -841,26 +1055,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6978B76C-41D6-4CB8-BB5A-CE3CBB65EA6D}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDA40C-CB43-498D-A2ED-A0851564593B}">
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -869,6 +1258,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6978B76C-41D6-4CB8-BB5A-CE3CBB65EA6D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1988A2C0-E26B-4053-9887-74900EAFFAF5}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -876,59 +1293,24 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A3F6A9-43ED-49B3-9AC1-A223C8D04358}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -944,9 +1326,9 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -972,7 +1354,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1008,25 +1390,25 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1041,26 +1423,26 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>

</xml_diff>